<commit_message>
Atualizando arquivos de teste
</commit_message>
<xml_diff>
--- a/automatize_me/resources/arquivos/arquivo.xlsx
+++ b/automatize_me/resources/arquivos/arquivo.xlsx
@@ -4,6 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Planilha_01" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha_02" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -594,4 +595,172 @@
     <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>CAMPO_01</v>
+      </c>
+      <c r="B1" t="str">
+        <v>CAMPO_02</v>
+      </c>
+      <c r="C1" t="str">
+        <v>CAMPO_02</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>VALOR_01_01</v>
+      </c>
+      <c r="B2" t="str">
+        <v>VALOR_02_1</v>
+      </c>
+      <c r="C2" t="str">
+        <v>VALOR_03_1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>VALOR_01_2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>VALOR_02_2</v>
+      </c>
+      <c r="C3" t="str">
+        <v>VALOR_03_2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>VALOR_01_3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>VALOR_02_3</v>
+      </c>
+      <c r="C4" t="str">
+        <v>VALOR_03_3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>VALOR_01_4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>VALOR_02_4</v>
+      </c>
+      <c r="C5" t="str">
+        <v>VALOR_03_4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>VALOR_01_5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>VALOR_02_5</v>
+      </c>
+      <c r="C6" t="str">
+        <v>VALOR_03_5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>VALOR_01_6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>VALOR_02_6</v>
+      </c>
+      <c r="C7" t="str">
+        <v>VALOR_03_6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>VALOR_01_7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>VALOR_02_7</v>
+      </c>
+      <c r="C8" t="str">
+        <v>VALOR_03_7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>VALOR_01_8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>VALOR_02_8</v>
+      </c>
+      <c r="C9" t="str">
+        <v>VALOR_03_8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>VALOR_01_9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>VALOR_02_9</v>
+      </c>
+      <c r="C10" t="str">
+        <v>VALOR_03_9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>VALOR_01_10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>VALOR_02_10</v>
+      </c>
+      <c r="C11" t="str">
+        <v>VALOR_03_10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>VALOR_01_11</v>
+      </c>
+      <c r="B12" t="str">
+        <v>VALOR_02_11</v>
+      </c>
+      <c r="C12" t="str">
+        <v>VALOR_03_11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>VALOR_01_12</v>
+      </c>
+      <c r="B13" t="str">
+        <v>VALOR_02_12</v>
+      </c>
+      <c r="C13" t="str">
+        <v>VALOR_03_12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>VALOR_01_13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>VALOR_02_13</v>
+      </c>
+      <c r="C14" t="str">
+        <v>VALOR_03_13</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C14"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>